<commit_message>
updated operation book for prefetch.  fixed bookmarks
</commit_message>
<xml_diff>
--- a/docs/avail-bundle.xlsx
+++ b/docs/avail-bundle.xlsx
@@ -410,7 +410,7 @@
     <t>Bundle.entry</t>
   </si>
   <si>
-    <t>Entry Slice</t>
+    <t>entry-slices</t>
   </si>
   <si>
     <t>Entry in the bundle - will have a resource, or information</t>
@@ -687,10 +687,10 @@
     <t>For a POST/PUT operation, this is the equivalent outcome that would be returned for prefer = operationoutcome - except that the resource is always returned whether or not the outcome is returned.</t>
   </si>
   <si>
-    <t>Appt Slice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appointment {http://fhir.org/guides/argonaut-scheduling/StructureDefinition/appt-output}
+    <t>entry-appt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment {http://fhir.org/guides/argonaut-scheduling/StructureDefinition/argo-appt}
 </t>
   </si>
   <si>
@@ -707,7 +707,7 @@
     <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="match"/&gt;</t>
   </si>
   <si>
-    <t>OO Slice</t>
+    <t>entry-oo</t>
   </si>
   <si>
     <t xml:space="preserve">OperationOutcome
@@ -892,7 +892,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="39.65234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="21.96875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>

</xml_diff>